<commit_message>
adding the new pilots from surprise pilot 8 to new attention and school pilots
</commit_message>
<xml_diff>
--- a/Gorilla_tasks_surprise_project.xlsx
+++ b/Gorilla_tasks_surprise_project.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marjan/Desktop/aim_lab_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7E248A6-8CE4-0742-9454-749108563BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CBAA4F-63CB-7A45-8D2F-D4C386D3789C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31880" yWindow="1340" windowWidth="34560" windowHeight="18800" xr2:uid="{DC324ADB-B303-4648-BE43-7DA8A6AC98AA}"/>
+    <workbookView xWindow="29880" yWindow="660" windowWidth="34340" windowHeight="20480" activeTab="1" xr2:uid="{DC324ADB-B303-4648-BE43-7DA8A6AC98AA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="old_pilots" sheetId="1" r:id="rId1"/>
+    <sheet name="Surprise_pilots_adults" sheetId="3" r:id="rId2"/>
+    <sheet name="Attention_pilots_adults" sheetId="4" r:id="rId3"/>
+    <sheet name="Surprise_pilots_schools" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="233">
   <si>
     <t>Study_links</t>
   </si>
@@ -425,12 +428,365 @@
   <si>
     <t>18/10/2023-21/10/2023</t>
   </si>
+  <si>
+    <t>Pilot_number</t>
+  </si>
+  <si>
+    <t>attention_pilot_1</t>
+  </si>
+  <si>
+    <t>attention_pilot_2</t>
+  </si>
+  <si>
+    <t>abbreviation_file_names</t>
+  </si>
+  <si>
+    <t>study_description</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/project/118148</t>
+  </si>
+  <si>
+    <t>surprise_pilot_6</t>
+  </si>
+  <si>
+    <t>surprise_pilot_7</t>
+  </si>
+  <si>
+    <t>surprise_pilot_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">surprise_pilot_9 </t>
+  </si>
+  <si>
+    <t>surprise_pilot_10</t>
+  </si>
+  <si>
+    <t>surprise_pilot_11</t>
+  </si>
+  <si>
+    <t>surprise_pilot_12</t>
+  </si>
+  <si>
+    <t>surprise_pilot_13</t>
+  </si>
+  <si>
+    <t>school_pilot_1</t>
+  </si>
+  <si>
+    <t>Prolific_fdbk_nrnd_bigger_w_YPAG_changes_w_video_change_anxietyQn</t>
+  </si>
+  <si>
+    <t>Prolific_fdbk_nrnd_bigger_w_YPAG_changes_with_video (Clone)</t>
+  </si>
+  <si>
+    <t>SUP_PRF_pilot_fdbk_bignrnd_YPAG_vid_anxQ</t>
+  </si>
+  <si>
+    <t>task_link</t>
+  </si>
+  <si>
+    <t>experiment_link</t>
+  </si>
+  <si>
+    <t>via Discord, direct Gorilla link</t>
+  </si>
+  <si>
+    <t>Elena Bagdades</t>
+  </si>
+  <si>
+    <t>Marjan biria</t>
+  </si>
+  <si>
+    <t>task_name</t>
+  </si>
+  <si>
+    <t>surprise_task_PE_feedback_YPAG_video_re-inroduced </t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/task/728998/editor?version=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clone of pilot 10 but changed the anxiety question to 'How relaxed do you feel right now?' to see whether 1) change in valence (having bood mood and anxiety questions having the same positive valence), and 2) it is easier to check how relaxed someone is on a momentarily basis easier/more feasible compared to anxiety. </t>
+  </si>
+  <si>
+    <t>The anxiety question remained the same as surprise_pilot_10 (i.e. "how nervous/uncomfortable do you feel right now?" since the results in pilot 12 did not change the effect size, only the direction of the relationship; in this pilot we increased the size of the negaive PE, by subtracting 10 from one of the negative PE's we had before per judge. We still kept one big positive PE per judge as before.</t>
+  </si>
+  <si>
+    <t>Results/conclusions</t>
+  </si>
+  <si>
+    <t>the results in pilot 12 did not change the effect size, only the direction of the relationship between anxiety and subjective PE (it become +0.18 instead of ~ -0.18)</t>
+  </si>
+  <si>
+    <t>Cloned Pilot 10_added_bigger_negative_PE</t>
+  </si>
+  <si>
+    <t>Prolific_YPAG_changes_vid_bigger_pos_&amp;_neg_PE</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/project/119459</t>
+  </si>
+  <si>
+    <t>surprise_task_PE_feedback_YPAG_video_adults_bigger_neg_PE</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/task/736716/editor</t>
+  </si>
+  <si>
+    <t>Cloned Pilot 10 for Students</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/project/115563</t>
+  </si>
+  <si>
+    <t>surprise_task_PE_feedback_YPAG_video_re-introduced_students</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/task/726685/editor</t>
+  </si>
+  <si>
+    <t>Surprise_pilot_10 but adjusted for students, we have added a few debriefing questions at the end to see how students felt about the task and whether they thought it was AI generated or not; however, we plan to change these questions to have people give their answers about believability on a scale of 0-100</t>
+  </si>
+  <si>
+    <t>ongoing</t>
+  </si>
+  <si>
+    <t>Charlotte Burman</t>
+  </si>
+  <si>
+    <t>Elena Bagdades, Marjan Biria</t>
+  </si>
+  <si>
+    <t>Prolific_attention_w_video_no_feedback_picture_disappears</t>
+  </si>
+  <si>
+    <t>Prolific_fdbk_nrnd_bigger_w_YPAG_changes_with_video (Clone) (Clone)</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/project/115369</t>
+  </si>
+  <si>
+    <t>surprise_task_PE_feedback_YPAG_video_re-inroduced (Clone) (Clone)</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/task/712861/editor</t>
+  </si>
+  <si>
+    <t>we have devided the surprise task into two blocks, without feedback and instructed participants to either pay external attention (first block with 24 trials) or internal attention (with 24 trials). The only data we collected from participants were mood and anxiety ratings. The stimuli they had to describe was presented for 4 seconds before they had to explain it to the other player/judge</t>
+  </si>
+  <si>
+    <t>The results were not very clear, so we decided to park this pilot while we optimise the surprise pilot, must come back to this later)</t>
+  </si>
+  <si>
+    <t>slight relationship between mood, anxiety and attention conditions, but not significant, we also did not counter balance the orders which is why we did the next pilot</t>
+  </si>
+  <si>
+    <r>
+      <t>Elena Bagdades</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Charlotte Burman, Marjan Biria</t>
+  </si>
+  <si>
+    <t>Prolific_attention_w_video_no_feedback_countbalanced</t>
+  </si>
+  <si>
+    <t>Prolific_fdbk_nrnd_bigger_w_YPAG_changes_with_video (Clone) (Clone) (Clone)</t>
+  </si>
+  <si>
+    <t>Surprise_Task_Attention_counterbalanced</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/project/117624</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/task/725729/editor</t>
+  </si>
+  <si>
+    <t>13/12/2023-14/12/2023</t>
+  </si>
+  <si>
+    <t>Marjan Biria, Naomi Tromans</t>
+  </si>
+  <si>
+    <t>SUP_PRF_pilot_no_fdbk_attention_vid</t>
+  </si>
+  <si>
+    <t>SUP_PRF_pilot_no_fdbk_attention_vid_cbal</t>
+  </si>
+  <si>
+    <t>The data quality was much better than Mturk, on Mturk people gave lots of random replies, where we had flat lines for ratings and no relationship between historgam and prediction. So we decided to keep using Mturk, Testable Minds participants' pool was also much smaller than Prolific and it would take a long time to collect data.</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/task/667140/editor?version=7</t>
+  </si>
+  <si>
+    <t>surprise_task_random_feedback </t>
+  </si>
+  <si>
+    <t>Marjan Biria</t>
+  </si>
+  <si>
+    <t>Charlotte Burman, Elena Bagdades, Isobel Ridler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">similar to the above except we counter balanced the order of internal vs external attention and had the picture presentation to be similar to the surprise task (not shown before they had to describe it, which may not have been a good idea, it may be worth re-introducing it in a next pilot!); another change we had made here which is only seen in the spreadsheet and output files, is how the mood and anxiety answers are numbered in the instructions and practice (right before they start the experiment), we named it Anxiety (practice), Mood (practice), </t>
+  </si>
+  <si>
+    <t>2 people did start but could not do the study due to various reasons (internet connection or other reasons), there were 7 people who could not continue due to an issue from Gorilla's side, it was related to the spreadsheet not being updated automatically which did happen before</t>
+  </si>
+  <si>
+    <t>SUP_PRF_pilot_vid_big_pos_neg_PE</t>
+  </si>
+  <si>
+    <t>go back to messahes on Prolific to check for pilots 6-11</t>
+  </si>
+  <si>
+    <t>modality</t>
+  </si>
+  <si>
+    <t>video + audio</t>
+  </si>
+  <si>
+    <t>typing, no video</t>
+  </si>
+  <si>
+    <t>repeating the same study as pilot_fdbk_nrand_typing_novid but with bigger positive PE (creating a list of numbers between 12 to 20, selecting randomly a number and adding it to one of the feedback values we had produced before), once per judge; the first 5 people until 20th Oct noon had high social anxiety, the rest included anyone without the screening to speed up the testing</t>
+  </si>
+  <si>
+    <t>surprise_task_PE_feedback (Clone)</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/task/682150/editor?version=4</t>
+  </si>
+  <si>
+    <t>The effect size did increase for the relationship between mood/anxiety and subjective PE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive PE: we selected numbers from a normal distribution ranging from 12-20, added this number to the mean of the histogram.  Negative PE: we selected numbers from a normal distribution ranging from 12-20, subtracted this number to the mean of the histogram.  Big positive PE: Per judge, we added 10 to the biggest positive feedback we had generated before. Big negative PE: Per judge, we subtracted 10 to the smallest negative feedback we had generated before. Neutral PE:  we added -1, 0, 1 to the mean of the histograms </t>
+  </si>
+  <si>
+    <t>TO BE ADDED: timings (ISI, screens), for defualt tasks generating PE, with a distribution of m=12, min-max=12-20</t>
+  </si>
+  <si>
+    <t>Prolific_non_random_feedback_biggest_PE</t>
+  </si>
+  <si>
+    <t>surprise_Prolific_PE_feedback_novideo (Clone) (Clone)</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/project/111504</t>
+  </si>
+  <si>
+    <t>surprise_task_PE_feedback_biggestPE</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/task/690668/editor</t>
+  </si>
+  <si>
+    <t>smaller effect size when having one maximum PE per judge (feedback between 90-100), so one bigger PE gave us better results</t>
+  </si>
+  <si>
+    <t>incorporating feedback from YPAG (OCT 2023); We used the task version from pilot 7, as this showed better relationship between PE, anxiety and mood. We took some of the
+feedback we received from the YPAG members into account here: 1) added a progress bar so that people
+know how much longer is left from the session, 2) make timing of feedback presentation more variable
+(1-4s) to make it more believable that someone is writing the rating, 3) changing the way we ask the
+question about emotion ratings, instead of “at the moment” we ask “right now”: how happy do you feel
+right now, 4) we have replaced the word “anxious” with “nervous or uncomfortable”: how nervous or
+uncomfortable fo you feel at the moment? Participants were not screened for social anxiety.</t>
+  </si>
+  <si>
+    <t>Prolific_fdbk_nrnd_bigger_w_YPAG_changes</t>
+  </si>
+  <si>
+    <t>SUP_PRF_pilot_fdbk_bignrnd_typ_YPAG</t>
+  </si>
+  <si>
+    <t>SUP_PRF_pilot_fdbk_bignrnd_YPAG_vid/SUP_PRF_pilot_fdbk_bignrnd_YPAG_vid_v5</t>
+  </si>
+  <si>
+    <t>SUP_PRF_pilot_fdbk_bignrnd_YPAG_vid/SUP_PRF_pilot_fdbk_bignrnd_YPAG_vid_v7</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/task/693731/editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">surprise_task_PE_feedback (Clone) (Clone) </t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/project/112181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feedback was calculated this way: </t>
+  </si>
+  <si>
+    <t>results relatively similar to before, similar effect sizes for the relationship between anxiety/mood and subjtive PE (although a bit smaller for anxiety, so we wanted to see in next pilot whether adding the video would change this)</t>
+  </si>
+  <si>
+    <t>Same version of the task as pilot 9 (prediction, bigger feedback, replacing anxiety with nervous/uncomfortable) + re-introducing  video/audio</t>
+  </si>
+  <si>
+    <t>The data very similar to pilot 7</t>
+  </si>
+  <si>
+    <t>notes: 1) Gorilla does not allow recording audio and video files separately, so we have to always make sure
+“audio” is not ticked in the setting and we only choose the video. Video file will include the audio, otherwise,
+audio files will overwrite the video files. 2) The second issue is that video files are only 4s approximately
+despite the trials being 15s, Elena is in contact with the Gorilla support team to resolve this issue. Although
+it does not impact the current data, we do want to solve it for the actual experiment in case someone wants
+to analyse those video data in the future.</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>We repeated the task (as the one on Mturk) with non-random feedback on Prolific to see whether the data quality would be better; repeating the same study as pilot_fdbk_rand_typing_novid but on Prolific</t>
+  </si>
+  <si>
+    <t>Prolific_fdbk_nrnd_bigger_w_YPAG_changes_with_video</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/project/113101</t>
+  </si>
+  <si>
+    <t>surprise_task_PE_feedback_YPAG_video_re-inroduced</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/task/698788/editor</t>
+  </si>
+  <si>
+    <t>10/11/2023-11/11/2023</t>
+  </si>
+  <si>
+    <t>22/11/2023-28/11/2023</t>
+  </si>
+  <si>
+    <t>Charlotte Burman, Elena Bagdades, Naomi Tromans</t>
+  </si>
+  <si>
+    <t>In this pilot we screened people for high social anxiety. The task itself, is the same as pilot 10 (re-introducing
+the video). During the screening, we selected people scoring 6 or higher for mini.</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/task/698788/editor?version=6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -466,13 +822,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -488,7 +868,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -502,6 +882,25 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -821,21 +1220,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37628269-7621-9840-90B1-E7E9F3D7C90A}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="61.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="47.6640625" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="37.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" style="3" customWidth="1"/>
     <col min="8" max="8" width="22.83203125" style="3" customWidth="1"/>
-    <col min="9" max="11" width="18" style="3" customWidth="1"/>
+    <col min="9" max="9" width="30.5" style="3" customWidth="1"/>
+    <col min="10" max="11" width="18" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -1649,7 +2049,861 @@
     <hyperlink ref="B18" r:id="rId37" xr:uid="{F7876E38-8B28-E64C-BD43-8BA1D23A4B96}"/>
     <hyperlink ref="B17" r:id="rId38" display="https://app.gorilla.sc/admin/experiment/143018" xr:uid="{9F128445-1BDD-814A-9B65-8F18DAF8B76D}"/>
     <hyperlink ref="A17" r:id="rId39" display="https://app.gorilla.sc/admin/project/105102" xr:uid="{B75F35D7-3BCC-0547-BB45-DEB230D5F30A}"/>
+    <hyperlink ref="D20" r:id="rId40" xr:uid="{EB94B830-4844-BD4A-B600-44C398D69267}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEF90CF-4CB5-8A43-AC17-CCF9610BD222}">
+  <dimension ref="A1:R12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+    <col min="4" max="5" width="42.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" customWidth="1"/>
+    <col min="9" max="10" width="16.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" style="3" customWidth="1"/>
+    <col min="13" max="14" width="21.1640625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="12" style="3" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="19.33203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+    </row>
+    <row r="2" spans="1:18" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="16"/>
+    </row>
+    <row r="3" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" t="s">
+        <v>187</v>
+      </c>
+      <c r="H5" t="s">
+        <v>186</v>
+      </c>
+      <c r="I5" t="s">
+        <v>223</v>
+      </c>
+      <c r="J5" t="s">
+        <v>185</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M5" s="3">
+        <v>20</v>
+      </c>
+      <c r="N5" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6" t="s">
+        <v>196</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G6" t="s">
+        <v>198</v>
+      </c>
+      <c r="H6" t="s">
+        <v>199</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="J6" t="s">
+        <v>200</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M6" s="3">
+        <v>37</v>
+      </c>
+      <c r="N6" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7" t="s">
+        <v>204</v>
+      </c>
+      <c r="E7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F7" t="s">
+        <v>205</v>
+      </c>
+      <c r="G7" t="s">
+        <v>206</v>
+      </c>
+      <c r="H7" t="s">
+        <v>207</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="J7" t="s">
+        <v>208</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M7" s="3">
+        <v>41</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="4">
+        <v>45226</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8" t="s">
+        <v>211</v>
+      </c>
+      <c r="E8" t="s">
+        <v>196</v>
+      </c>
+      <c r="F8" t="s">
+        <v>216</v>
+      </c>
+      <c r="G8" t="s">
+        <v>215</v>
+      </c>
+      <c r="H8" t="s">
+        <v>214</v>
+      </c>
+      <c r="I8" t="s">
+        <v>209</v>
+      </c>
+      <c r="J8" t="s">
+        <v>218</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M8" s="3">
+        <v>37</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" s="4">
+        <v>45236</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" t="s">
+        <v>212</v>
+      </c>
+      <c r="E9" t="s">
+        <v>195</v>
+      </c>
+      <c r="F9" t="s">
+        <v>225</v>
+      </c>
+      <c r="G9" t="s">
+        <v>226</v>
+      </c>
+      <c r="H9" t="s">
+        <v>227</v>
+      </c>
+      <c r="I9" t="s">
+        <v>219</v>
+      </c>
+      <c r="J9" t="s">
+        <v>220</v>
+      </c>
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M9" s="3">
+        <v>39</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C10" t="s">
+        <v>224</v>
+      </c>
+      <c r="D10" t="s">
+        <v>213</v>
+      </c>
+      <c r="E10" t="s">
+        <v>195</v>
+      </c>
+      <c r="F10" t="s">
+        <v>225</v>
+      </c>
+      <c r="G10" t="s">
+        <v>147</v>
+      </c>
+      <c r="H10" t="s">
+        <v>232</v>
+      </c>
+      <c r="I10" t="s">
+        <v>231</v>
+      </c>
+      <c r="K10">
+        <v>7</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" t="s">
+        <v>140</v>
+      </c>
+      <c r="E11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F11" t="s">
+        <v>128</v>
+      </c>
+      <c r="G11" t="s">
+        <v>147</v>
+      </c>
+      <c r="H11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I11" t="s">
+        <v>149</v>
+      </c>
+      <c r="J11" t="s">
+        <v>152</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11" s="3">
+        <v>25</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" s="4">
+        <v>45278</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" t="s">
+        <v>192</v>
+      </c>
+      <c r="E12" t="s">
+        <v>195</v>
+      </c>
+      <c r="F12" t="s">
+        <v>155</v>
+      </c>
+      <c r="G12" t="s">
+        <v>156</v>
+      </c>
+      <c r="H12" t="s">
+        <v>157</v>
+      </c>
+      <c r="I12" t="s">
+        <v>150</v>
+      </c>
+      <c r="K12">
+        <v>5</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M12" s="16">
+        <v>29</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="O12" s="4">
+        <v>45303</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{50A62B91-99A1-3A43-B9B6-29B172BF77F2}"/>
+    <hyperlink ref="C6" r:id="rId2" display="https://app.gorilla.sc/admin/experiment/147683" xr:uid="{2F4E49B3-774A-834B-A1DD-0FE1BAF1F957}"/>
+    <hyperlink ref="F6" r:id="rId3" xr:uid="{828C53D0-439A-514B-AC6F-23045E714D0D}"/>
+    <hyperlink ref="H10" r:id="rId4" xr:uid="{0AB04F01-A831-1F40-8328-D99DF81352D7}"/>
+    <hyperlink ref="F10" r:id="rId5" xr:uid="{BF8B9C19-6CB0-284A-B7F4-4B76A7837FB5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0EBF7F-DB98-AC42-941C-7C09939411EE}">
+  <dimension ref="A1:R12"/>
+  <sheetViews>
+    <sheetView zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="5" width="22.1640625" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="26" customWidth="1"/>
+    <col min="10" max="10" width="18.5" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" customWidth="1"/>
+    <col min="13" max="13" width="21.83203125" customWidth="1"/>
+    <col min="14" max="14" width="14.5" customWidth="1"/>
+    <col min="15" max="15" width="15.1640625" customWidth="1"/>
+    <col min="16" max="16" width="19.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I2" t="s">
+        <v>171</v>
+      </c>
+      <c r="J2" t="s">
+        <v>173</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M2">
+        <v>29</v>
+      </c>
+      <c r="N2">
+        <v>45259</v>
+      </c>
+      <c r="O2" t="s">
+        <v>174</v>
+      </c>
+      <c r="P2" t="s">
+        <v>175</v>
+      </c>
+      <c r="R2" s="10"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G3" t="s">
+        <v>178</v>
+      </c>
+      <c r="H3" t="s">
+        <v>180</v>
+      </c>
+      <c r="I3" t="s">
+        <v>190</v>
+      </c>
+      <c r="J3" t="s">
+        <v>172</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3">
+        <v>58</v>
+      </c>
+      <c r="N3" t="s">
+        <v>181</v>
+      </c>
+      <c r="O3" t="s">
+        <v>144</v>
+      </c>
+      <c r="P3" t="s">
+        <v>182</v>
+      </c>
+      <c r="R3" s="10"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R4" s="10"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E12" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C34846-31F7-6D4F-84C1-025AA01B057C}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="4" max="5" width="24.5" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" customWidth="1"/>
+    <col min="8" max="10" width="17.1640625" customWidth="1"/>
+    <col min="11" max="11" width="20.5" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" customWidth="1"/>
+    <col min="13" max="13" width="21.33203125" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="15" max="15" width="17.5" customWidth="1"/>
+    <col min="16" max="16" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I2" t="s">
+        <v>162</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>143</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="O2" t="s">
+        <v>164</v>
+      </c>
+      <c r="P2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the pilot data and some scripts for pilot 13
</commit_message>
<xml_diff>
--- a/Gorilla_tasks_surprise_project.xlsx
+++ b/Gorilla_tasks_surprise_project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marjan/Desktop/aim_lab_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CBAA4F-63CB-7A45-8D2F-D4C386D3789C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A409447-0A1C-474D-8B4F-51BA3AA6C773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29880" yWindow="660" windowWidth="34340" windowHeight="20480" activeTab="1" xr2:uid="{DC324ADB-B303-4648-BE43-7DA8A6AC98AA}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="1" xr2:uid="{DC324ADB-B303-4648-BE43-7DA8A6AC98AA}"/>
   </bookViews>
   <sheets>
     <sheet name="old_pilots" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="236">
   <si>
     <t>Study_links</t>
   </si>
@@ -780,6 +780,15 @@
   </si>
   <si>
     <t>https://app.gorilla.sc/admin/task/698788/editor?version=6</t>
+  </si>
+  <si>
+    <t>biggest</t>
+  </si>
+  <si>
+    <t>bigger</t>
+  </si>
+  <si>
+    <t>normal_PE</t>
   </si>
 </sst>
 </file>
@@ -868,7 +877,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -885,19 +894,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2057,67 +2061,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEF90CF-4CB5-8A43-AC17-CCF9610BD222}">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.83203125" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" customWidth="1"/>
-    <col min="4" max="5" width="42.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" customWidth="1"/>
-    <col min="9" max="10" width="16.6640625" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" style="3" customWidth="1"/>
-    <col min="13" max="14" width="21.1640625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="12" style="3" customWidth="1"/>
-    <col min="16" max="16" width="14.33203125" style="3" customWidth="1"/>
-    <col min="17" max="17" width="19.33203125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="10.83203125" style="3"/>
+    <col min="3" max="4" width="48.5" customWidth="1"/>
+    <col min="5" max="5" width="73.6640625" customWidth="1"/>
+    <col min="6" max="6" width="42.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="10" max="11" width="16.6640625" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" style="3" customWidth="1"/>
+    <col min="14" max="15" width="21.1640625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="12" style="3" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="19.33203125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-    </row>
-    <row r="2" spans="1:18" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+    </row>
+    <row r="2" spans="1:19" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="16"/>
-    </row>
-    <row r="3" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>123</v>
       </c>
@@ -2127,50 +2115,51 @@
       <c r="C4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -2181,49 +2170,52 @@
         <v>114</v>
       </c>
       <c r="D5" t="s">
+        <v>235</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>196</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>115</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>187</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>186</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>223</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>185</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>3</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="M5" s="3">
+      <c r="N5" s="3">
         <v>20</v>
       </c>
-      <c r="N5" s="17" t="s">
+      <c r="O5" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="P5" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="Q5" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="R5" s="3" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>130</v>
       </c>
@@ -2234,49 +2226,52 @@
         <v>117</v>
       </c>
       <c r="D6" t="s">
+        <v>234</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>196</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" t="s">
         <v>118</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>198</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>199</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>200</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>3</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="M6" s="3">
+      <c r="N6" s="3">
         <v>37</v>
       </c>
-      <c r="N6" s="16" t="s">
+      <c r="O6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="R6" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>131</v>
       </c>
@@ -2286,47 +2281,51 @@
       <c r="C7" t="s">
         <v>204</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D7" t="s">
+        <v>233</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" t="s">
         <v>196</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>205</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>206</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>207</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>208</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>3</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="M7" s="3">
+      <c r="N7" s="3">
         <v>41</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="O7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="4">
+      <c r="P7" s="4">
         <v>45226</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="Q7" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="R7" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>132</v>
       </c>
@@ -2336,47 +2335,47 @@
       <c r="C8" t="s">
         <v>204</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>211</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>196</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>216</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>215</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>214</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>209</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>218</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="M8" s="3">
+      <c r="N8" s="3">
         <v>37</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="O8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="4">
+      <c r="P8" s="4">
         <v>45236</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="Q8" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="R8" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>133</v>
       </c>
@@ -2386,50 +2385,50 @@
       <c r="C9" t="s">
         <v>224</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>212</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>195</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>225</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>226</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>227</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>219</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>220</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>5</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="M9" s="3">
+      <c r="N9" s="3">
         <v>39</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="O9" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="P9" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="Q9" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="Q9" s="9" t="s">
+      <c r="R9" s="8" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -2439,38 +2438,38 @@
       <c r="C10" t="s">
         <v>224</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>213</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>195</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>225</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>147</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>232</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>231</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>7</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="O10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="P10" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>135</v>
       </c>
@@ -2480,50 +2479,50 @@
       <c r="C11" t="s">
         <v>139</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>140</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>195</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>128</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>147</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>148</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>149</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>152</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>2</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="M11" s="3">
+      <c r="N11" s="3">
         <v>25</v>
       </c>
-      <c r="N11" s="3" t="s">
+      <c r="O11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O11" s="4">
+      <c r="P11" s="4">
         <v>45278</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="Q11" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="Q11" s="3" t="s">
+      <c r="R11" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>136</v>
       </c>
@@ -2533,53 +2532,53 @@
       <c r="C12" t="s">
         <v>154</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>192</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>195</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>155</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>156</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>157</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>150</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>5</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="M12" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="M12" s="16">
+      <c r="N12" s="3">
         <v>29</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="O12" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="O12" s="4">
+      <c r="P12" s="4">
         <v>45303</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="Q12" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="Q12" s="3" t="s">
+      <c r="R12" s="3" t="s">
         <v>144</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1" xr:uid="{50A62B91-99A1-3A43-B9B6-29B172BF77F2}"/>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{50A62B91-99A1-3A43-B9B6-29B172BF77F2}"/>
     <hyperlink ref="C6" r:id="rId2" display="https://app.gorilla.sc/admin/experiment/147683" xr:uid="{2F4E49B3-774A-834B-A1DD-0FE1BAF1F957}"/>
-    <hyperlink ref="F6" r:id="rId3" xr:uid="{828C53D0-439A-514B-AC6F-23045E714D0D}"/>
-    <hyperlink ref="H10" r:id="rId4" xr:uid="{0AB04F01-A831-1F40-8328-D99DF81352D7}"/>
-    <hyperlink ref="F10" r:id="rId5" xr:uid="{BF8B9C19-6CB0-284A-B7F4-4B76A7837FB5}"/>
+    <hyperlink ref="G6" r:id="rId3" xr:uid="{828C53D0-439A-514B-AC6F-23045E714D0D}"/>
+    <hyperlink ref="I10" r:id="rId4" xr:uid="{0AB04F01-A831-1F40-8328-D99DF81352D7}"/>
+    <hyperlink ref="G10" r:id="rId5" xr:uid="{BF8B9C19-6CB0-284A-B7F4-4B76A7837FB5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2670,7 +2669,7 @@
       <c r="C2" t="s">
         <v>167</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" t="s">
         <v>183</v>
       </c>
       <c r="E2" t="s">
@@ -2679,7 +2678,7 @@
       <c r="F2" t="s">
         <v>168</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" t="s">
         <v>169</v>
       </c>
       <c r="H2" t="s">
@@ -2709,7 +2708,7 @@
       <c r="P2" t="s">
         <v>175</v>
       </c>
-      <c r="R2" s="10"/>
+      <c r="R2" s="9"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -2718,10 +2717,10 @@
       <c r="B3" t="s">
         <v>176</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" t="s">
         <v>177</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" t="s">
         <v>184</v>
       </c>
       <c r="E3" t="s">
@@ -2760,16 +2759,16 @@
       <c r="P3" t="s">
         <v>182</v>
       </c>
-      <c r="R3" s="10"/>
+      <c r="R3" s="9"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="R4" s="10"/>
+      <c r="R4" s="9"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E12" s="2"/>

</xml_diff>

<commit_message>
updated the pilot info
</commit_message>
<xml_diff>
--- a/Gorilla_tasks_surprise_project.xlsx
+++ b/Gorilla_tasks_surprise_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marjan/Desktop/aim_lab_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A409447-0A1C-474D-8B4F-51BA3AA6C773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E591F824-2BAD-7946-8645-5869D2B314DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="1" xr2:uid="{DC324ADB-B303-4648-BE43-7DA8A6AC98AA}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="241">
   <si>
     <t>Study_links</t>
   </si>
@@ -629,12 +629,6 @@
     <t>The data quality was much better than Mturk, on Mturk people gave lots of random replies, where we had flat lines for ratings and no relationship between historgam and prediction. So we decided to keep using Mturk, Testable Minds participants' pool was also much smaller than Prolific and it would take a long time to collect data.</t>
   </si>
   <si>
-    <t>https://app.gorilla.sc/admin/task/667140/editor?version=7</t>
-  </si>
-  <si>
-    <t>surprise_task_random_feedback </t>
-  </si>
-  <si>
     <t>Marjan Biria</t>
   </si>
   <si>
@@ -782,13 +776,34 @@
     <t>https://app.gorilla.sc/admin/task/698788/editor?version=6</t>
   </si>
   <si>
-    <t>biggest</t>
-  </si>
-  <si>
-    <t>bigger</t>
-  </si>
-  <si>
     <t>normal_PE</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/project/108317</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/task/668808/editor?version=9</t>
+  </si>
+  <si>
+    <t>surprise_task_PE_feedback </t>
+  </si>
+  <si>
+    <t>SUP_PRF_pilot_fdbk_bignrnd_typ</t>
+  </si>
+  <si>
+    <t>SUP_PRF_pilot_fdbk_biggestnrnd_typ</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>bigger positive</t>
+  </si>
+  <si>
+    <t>biggest positive</t>
+  </si>
+  <si>
+    <t>bigger positive and negative</t>
   </si>
 </sst>
 </file>
@@ -877,7 +892,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -907,6 +922,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2064,7 +2081,7 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2087,7 +2104,7 @@
   <sheetData>
     <row r="1" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
@@ -2099,10 +2116,10 @@
     </row>
     <row r="2" spans="1:19" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -2115,12 +2132,14 @@
       <c r="C4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>237</v>
+      </c>
       <c r="E4" s="2" t="s">
         <v>126</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>142</v>
@@ -2147,7 +2166,7 @@
         <v>2</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>3</v>
@@ -2167,28 +2186,28 @@
         <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>235</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>103</v>
+        <v>231</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>102</v>
       </c>
       <c r="F5" t="s">
-        <v>196</v>
-      </c>
-      <c r="G5" t="s">
-        <v>115</v>
+        <v>194</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>232</v>
       </c>
       <c r="H5" t="s">
-        <v>187</v>
+        <v>234</v>
       </c>
       <c r="I5" t="s">
-        <v>186</v>
+        <v>233</v>
       </c>
       <c r="J5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="K5" t="s">
         <v>185</v>
@@ -2203,16 +2222,16 @@
         <v>20</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>111</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
@@ -2226,28 +2245,28 @@
         <v>117</v>
       </c>
       <c r="D6" t="s">
-        <v>234</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>112</v>
+        <v>238</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>235</v>
       </c>
       <c r="F6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G6" t="s">
         <v>118</v>
       </c>
       <c r="H6" t="s">
+        <v>196</v>
+      </c>
+      <c r="I6" t="s">
+        <v>197</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="K6" t="s">
         <v>198</v>
-      </c>
-      <c r="I6" t="s">
-        <v>199</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="K6" t="s">
-        <v>200</v>
       </c>
       <c r="L6">
         <v>3</v>
@@ -2265,7 +2284,7 @@
         <v>122</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="R6" s="3" t="s">
         <v>32</v>
@@ -2276,32 +2295,34 @@
         <v>131</v>
       </c>
       <c r="B7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D7" t="s">
+        <v>239</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="F7" t="s">
+        <v>194</v>
+      </c>
+      <c r="G7" t="s">
         <v>203</v>
       </c>
-      <c r="C7" t="s">
+      <c r="H7" t="s">
         <v>204</v>
       </c>
-      <c r="D7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" t="s">
-        <v>196</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>205</v>
-      </c>
-      <c r="H7" t="s">
-        <v>206</v>
-      </c>
-      <c r="I7" t="s">
-        <v>207</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>108</v>
       </c>
       <c r="K7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="L7">
         <v>3</v>
@@ -2319,7 +2340,7 @@
         <v>45226</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="R7" s="3" t="s">
         <v>144</v>
@@ -2330,31 +2351,34 @@
         <v>132</v>
       </c>
       <c r="B8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C8" t="s">
-        <v>204</v>
+        <v>202</v>
+      </c>
+      <c r="D8" t="s">
+        <v>238</v>
       </c>
       <c r="E8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H8" t="s">
+        <v>213</v>
+      </c>
+      <c r="I8" t="s">
+        <v>212</v>
+      </c>
+      <c r="J8" t="s">
+        <v>207</v>
+      </c>
+      <c r="K8" t="s">
         <v>216</v>
-      </c>
-      <c r="H8" t="s">
-        <v>215</v>
-      </c>
-      <c r="I8" t="s">
-        <v>214</v>
-      </c>
-      <c r="J8" t="s">
-        <v>209</v>
-      </c>
-      <c r="K8" t="s">
-        <v>218</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>69</v>
@@ -2380,31 +2404,34 @@
         <v>133</v>
       </c>
       <c r="B9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D9" t="s">
+        <v>238</v>
+      </c>
+      <c r="E9" t="s">
+        <v>210</v>
+      </c>
+      <c r="F9" t="s">
+        <v>193</v>
+      </c>
+      <c r="G9" t="s">
+        <v>223</v>
+      </c>
+      <c r="H9" t="s">
         <v>224</v>
       </c>
-      <c r="C9" t="s">
-        <v>224</v>
-      </c>
-      <c r="E9" t="s">
-        <v>212</v>
-      </c>
-      <c r="F9" t="s">
-        <v>195</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>225</v>
       </c>
-      <c r="H9" t="s">
-        <v>226</v>
-      </c>
-      <c r="I9" t="s">
-        <v>227</v>
-      </c>
       <c r="J9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="L9">
         <v>5</v>
@@ -2416,16 +2443,16 @@
         <v>39</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="P9" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="R9" s="8" t="s">
         <v>228</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="R9" s="8" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
@@ -2433,28 +2460,31 @@
         <v>134</v>
       </c>
       <c r="B10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C10" t="s">
-        <v>224</v>
+        <v>222</v>
+      </c>
+      <c r="D10" t="s">
+        <v>238</v>
       </c>
       <c r="E10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H10" t="s">
         <v>147</v>
       </c>
       <c r="I10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="L10">
         <v>7</v>
@@ -2466,7 +2496,7 @@
         <v>14</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
@@ -2479,11 +2509,14 @@
       <c r="C11" t="s">
         <v>139</v>
       </c>
+      <c r="D11" t="s">
+        <v>238</v>
+      </c>
       <c r="E11" t="s">
         <v>140</v>
       </c>
       <c r="F11" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G11" t="s">
         <v>128</v>
@@ -2532,11 +2565,14 @@
       <c r="C12" t="s">
         <v>154</v>
       </c>
+      <c r="D12" t="s">
+        <v>240</v>
+      </c>
       <c r="E12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G12" t="s">
         <v>155</v>
@@ -2560,7 +2596,7 @@
         <v>29</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="P12" s="4">
         <v>45303</v>
@@ -2623,7 +2659,7 @@
         <v>126</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>142</v>
@@ -2673,7 +2709,7 @@
         <v>183</v>
       </c>
       <c r="E2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F2" t="s">
         <v>168</v>
@@ -2724,7 +2760,7 @@
         <v>184</v>
       </c>
       <c r="E3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F3" t="s">
         <v>179</v>
@@ -2736,7 +2772,7 @@
         <v>180</v>
       </c>
       <c r="I3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J3" t="s">
         <v>172</v>
@@ -2816,7 +2852,7 @@
         <v>126</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>142</v>
@@ -2866,7 +2902,7 @@
         <v>163</v>
       </c>
       <c r="E2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F2" t="s">
         <v>159</v>

</xml_diff>

<commit_message>
updating recruitment info for all pilots
</commit_message>
<xml_diff>
--- a/Gorilla_tasks_surprise_project.xlsx
+++ b/Gorilla_tasks_surprise_project.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marjan/Desktop/aim_lab_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucjuagd_ucl_ac_uk/Documents/Documents/GitHub/aim_lab_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDB4E16-5207-A142-A9AE-6AADBE90B02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D17E5BA8-1333-49FC-A2F2-6D822B61540E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36340" yWindow="1340" windowWidth="29400" windowHeight="16680" activeTab="1" xr2:uid="{DC324ADB-B303-4648-BE43-7DA8A6AC98AA}"/>
   </bookViews>
@@ -23,22 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="340">
   <si>
     <t>Study_links</t>
   </si>
@@ -1008,6 +998,99 @@
   </si>
   <si>
     <t>04/03/2024-05/03/2024</t>
+  </si>
+  <si>
+    <t>surprose_pilot_20</t>
+  </si>
+  <si>
+    <t>surprose_pilot_21</t>
+  </si>
+  <si>
+    <t>surprose_pilot_22</t>
+  </si>
+  <si>
+    <t>surprise_pilot_20</t>
+  </si>
+  <si>
+    <t>surprise_pilot_21</t>
+  </si>
+  <si>
+    <t>surprise_pilot_22</t>
+  </si>
+  <si>
+    <t>new pred questions, second one after feedback, hist only early</t>
+  </si>
+  <si>
+    <t xml:space="preserve">second pred question, appears after the feedback </t>
+  </si>
+  <si>
+    <t>SUP_PRF_p20_vid_bigPE_2pred_afterfdbk_nohist_4jud</t>
+  </si>
+  <si>
+    <t>surprise_task_bigger_pos_PE_vid_adults_newnarrative_old_judges_new_qns_after_fdbk_hist_early_only</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/task/793630/editor</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/experiment/171533/design</t>
+  </si>
+  <si>
+    <t>15/03/24-18/03/24</t>
+  </si>
+  <si>
+    <t>same as pilot 19 but the second prediction question appears after feedback: "You do you think you did?"</t>
+  </si>
+  <si>
+    <t>real judges, no seond pred</t>
+  </si>
+  <si>
+    <t xml:space="preserve">replaced judge pictures with pictures of real people, removed 2nd pred </t>
+  </si>
+  <si>
+    <t>SUP_PRF_p21_vid_bigPE_nohist_newjud</t>
+  </si>
+  <si>
+    <t>3, 4</t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/experiment/172741/design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">surprise_task_bigger_pos_PE_vid_adults_newnarrative_real_judges_new_qn_hist_early_only </t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/task/799523/editor</t>
+  </si>
+  <si>
+    <t>replaced judge pictures with real pictures, removed second pred, histogram only shown once per judge</t>
+  </si>
+  <si>
+    <t>22/03/24-29/03/24</t>
+  </si>
+  <si>
+    <t>12/03/24-14/04/24</t>
+  </si>
+  <si>
+    <t>surprise_pilot_22 (Clone)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changed anxiety question and added embarrassement qn </t>
+  </si>
+  <si>
+    <t>anxiety qn became ("How nervous would you feel to speak to this person again?"); embarrassment qn (How embarrassed do you feel right now?")</t>
+  </si>
+  <si>
+    <t>SUP_PRF_p22_vid_bigPE_nohist_newjud_2anxQ</t>
+  </si>
+  <si>
+    <t>surprise_task_bigger_pos_PE_vid_adults_real_judges_new_qn_hist_early_only_2anxQns (gorilla.sc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">surprise_task_bigger_pos_PE_vid_adults_real_judges_new_qn_hist_early_only_2anxQns </t>
+  </si>
+  <si>
+    <t>https://app.gorilla.sc/admin/experiment/175513/design</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1127,6 +1210,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1448,7 +1532,7 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="47.6640625" customWidth="1"/>
     <col min="2" max="2" width="45.83203125" style="3" customWidth="1"/>
@@ -2230,7 +2314,7 @@
       <c r="C25" s="5"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K25">
+  <sortState ref="A2:K25">
     <sortCondition ref="G1:G25"/>
   </sortState>
   <hyperlinks>
@@ -2281,13 +2365,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEF90CF-4CB5-8A43-AC17-CCF9610BD222}">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="27.83203125" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
@@ -3230,7 +3314,175 @@
       </c>
     </row>
     <row r="19" spans="1:20">
-      <c r="G19" s="13"/>
+      <c r="A19" t="s">
+        <v>309</v>
+      </c>
+      <c r="B19" t="s">
+        <v>312</v>
+      </c>
+      <c r="C19" t="s">
+        <v>312</v>
+      </c>
+      <c r="D19" t="s">
+        <v>234</v>
+      </c>
+      <c r="E19" t="s">
+        <v>315</v>
+      </c>
+      <c r="F19" t="s">
+        <v>316</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="H19" t="s">
+        <v>191</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="J19" t="s">
+        <v>318</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="N19">
+        <v>4</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P19" s="3">
+        <v>55</v>
+      </c>
+      <c r="Q19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="T19" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" t="s">
+        <v>310</v>
+      </c>
+      <c r="B20" t="s">
+        <v>313</v>
+      </c>
+      <c r="C20" t="s">
+        <v>313</v>
+      </c>
+      <c r="D20" t="s">
+        <v>234</v>
+      </c>
+      <c r="E20" t="s">
+        <v>323</v>
+      </c>
+      <c r="F20" t="s">
+        <v>324</v>
+      </c>
+      <c r="G20" t="s">
+        <v>325</v>
+      </c>
+      <c r="H20" t="s">
+        <v>191</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="J20" t="s">
+        <v>328</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="N20" t="s">
+        <v>326</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P20" s="3">
+        <v>37</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" t="s">
+        <v>311</v>
+      </c>
+      <c r="B21" t="s">
+        <v>314</v>
+      </c>
+      <c r="C21" t="s">
+        <v>333</v>
+      </c>
+      <c r="D21" t="s">
+        <v>234</v>
+      </c>
+      <c r="E21" t="s">
+        <v>334</v>
+      </c>
+      <c r="F21" t="s">
+        <v>335</v>
+      </c>
+      <c r="G21" t="s">
+        <v>336</v>
+      </c>
+      <c r="H21" t="s">
+        <v>191</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="J21" t="s">
+        <v>338</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P21" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>257</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3246,9 +3498,15 @@
     <hyperlink ref="K15" r:id="rId10" xr:uid="{02CC67ED-114B-4D0F-8E7A-AC02822C8E2E}"/>
     <hyperlink ref="K14" r:id="rId11" xr:uid="{6E661706-50E1-4EC0-B53A-1413591BB266}"/>
     <hyperlink ref="K17" r:id="rId12" xr:uid="{B77D67BA-31B8-4A4E-9728-3E41455D7DB1}"/>
+    <hyperlink ref="I19" r:id="rId13" xr:uid="{CABE5D4A-3230-4C2A-A58F-B3F85F20F8CB}"/>
+    <hyperlink ref="K19" r:id="rId14" xr:uid="{05C0F5C9-F697-4159-A5F1-CDB4D302E155}"/>
+    <hyperlink ref="I20" r:id="rId15" xr:uid="{E3A20808-1F30-46C7-967C-95859AE2BD3A}"/>
+    <hyperlink ref="K20" r:id="rId16" xr:uid="{8327E9AE-777E-419F-86AA-1211483EA88D}"/>
+    <hyperlink ref="K21" r:id="rId17" display="https://app.gorilla.sc/admin/task/812527/editor?version=6" xr:uid="{E96A5072-D9EE-42A2-9808-680185E6095F}"/>
+    <hyperlink ref="I21" r:id="rId18" xr:uid="{0083D627-8165-479C-B24A-9E5096F4BAEB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 
@@ -3260,7 +3518,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
@@ -3454,7 +3712,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
@@ -3576,12 +3834,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="e5a9619a-7000-4aea-a2bb-374d291ba315" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3832,17 +4089,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="e5a9619a-7000-4aea-a2bb-374d291ba315" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E99AFF9C-0561-42E5-88DF-7F2536EABBC5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7586151B-4E7D-4418-B659-2C4EEEFAD5DD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e5a9619a-7000-4aea-a2bb-374d291ba315"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="47378dc1-fef5-4e17-a461-02e6a7c158f1"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3867,18 +4134,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7586151B-4E7D-4418-B659-2C4EEEFAD5DD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E99AFF9C-0561-42E5-88DF-7F2536EABBC5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="e5a9619a-7000-4aea-a2bb-374d291ba315"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="47378dc1-fef5-4e17-a461-02e6a7c158f1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
moved data to folder
</commit_message>
<xml_diff>
--- a/Gorilla_tasks_surprise_project.xlsx
+++ b/Gorilla_tasks_surprise_project.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elena\OneDrive - University College London\Documents\GitHub\aim_lab_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elena\OneDrive - University College London\Desktop\GitHub\aim_lab_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="14_{829A784D-6E8F-4D11-8242-303D8D0BFC9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BD7EF8E-36FB-4DA6-BEB3-F0A6FBF1257B}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="14_{829A784D-6E8F-4D11-8242-303D8D0BFC9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A717278-0E04-4FDF-881F-D249CFF2D574}"/>
   <bookViews>
-    <workbookView xWindow="36340" yWindow="1340" windowWidth="29400" windowHeight="16680" activeTab="1" xr2:uid="{DC324ADB-B303-4648-BE43-7DA8A6AC98AA}"/>
+    <workbookView xWindow="36340" yWindow="1340" windowWidth="29400" windowHeight="16680" activeTab="2" xr2:uid="{DC324ADB-B303-4648-BE43-7DA8A6AC98AA}"/>
   </bookViews>
   <sheets>
     <sheet name="old_pilots" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="357">
   <si>
     <t>Study_links</t>
   </si>
@@ -1100,6 +1100,48 @@
   </si>
   <si>
     <t>correlation between anxiety/mood and subjPE improved from pilot 20</t>
+  </si>
+  <si>
+    <t>school_pilot_2</t>
+  </si>
+  <si>
+    <t>AMT_pilot_1</t>
+  </si>
+  <si>
+    <t>Folder_name</t>
+  </si>
+  <si>
+    <t>AMT_pilot_2</t>
+  </si>
+  <si>
+    <t>AMT_pilot_3</t>
+  </si>
+  <si>
+    <t>AMT_pilot_4</t>
+  </si>
+  <si>
+    <t>AMT_pilot_6</t>
+  </si>
+  <si>
+    <t>AMT_pilot_5</t>
+  </si>
+  <si>
+    <t>pilot_1</t>
+  </si>
+  <si>
+    <t>pilot_2</t>
+  </si>
+  <si>
+    <t>pilot_6</t>
+  </si>
+  <si>
+    <t>pilot_4</t>
+  </si>
+  <si>
+    <t>pilot_3</t>
+  </si>
+  <si>
+    <t>pilot_5</t>
   </si>
 </sst>
 </file>
@@ -1535,27 +1577,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37628269-7621-9840-90B1-E7E9F3D7C90A}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="47.6640625" customWidth="1"/>
-    <col min="2" max="2" width="45.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="37.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="22.83203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="30.5" style="3" customWidth="1"/>
-    <col min="10" max="11" width="18" style="3" customWidth="1"/>
+    <col min="2" max="3" width="45.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="37.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="22.83203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="30.5" style="3" customWidth="1"/>
+    <col min="11" max="12" width="18" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>91</v>
       </c>
@@ -1563,34 +1605,37 @@
         <v>36</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" s="5" t="s">
         <v>43</v>
       </c>
@@ -1598,35 +1643,38 @@
         <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>8</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>4</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="5" t="s">
         <v>46</v>
       </c>
@@ -1634,35 +1682,38 @@
         <v>56</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>2</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>3</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="5" t="s">
         <v>50</v>
       </c>
@@ -1670,35 +1721,38 @@
         <v>50</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>142</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <v>45196</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="5" t="s">
         <v>51</v>
       </c>
@@ -1706,35 +1760,38 @@
         <v>51</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>6</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>79</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="5" t="s">
         <v>52</v>
       </c>
@@ -1742,35 +1799,38 @@
         <v>75</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>5</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <v>3</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="5" t="s">
         <v>54</v>
       </c>
@@ -1778,35 +1838,38 @@
         <v>81</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>5</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="3">
         <v>4</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="5" t="s">
         <v>44</v>
       </c>
@@ -1814,32 +1877,33 @@
         <v>92</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="3">
         <v>0</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9" s="5" t="s">
         <v>42</v>
       </c>
@@ -1847,32 +1911,33 @@
         <v>7</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>1</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="3">
+      <c r="I9" s="3">
         <v>0</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10" s="5" t="s">
         <v>37</v>
       </c>
@@ -1880,32 +1945,33 @@
         <v>18</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <v>1</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="3">
+      <c r="I10" s="3">
         <v>0</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="K10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
@@ -1913,32 +1979,33 @@
         <v>29</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <v>1</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="3">
+      <c r="I11" s="3">
         <v>0</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="J11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="K11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="L11" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12" s="5" t="s">
         <v>33</v>
       </c>
@@ -1946,64 +2013,66 @@
         <v>33</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="3">
         <v>3</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="3">
+      <c r="I12" s="3">
         <v>0</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="J12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="K12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="L12" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="C13" s="5"/>
+      <c r="E13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="3">
         <v>4</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="3">
+      <c r="I13" s="3">
         <v>0</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="K13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="L13" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
@@ -2011,32 +2080,33 @@
         <v>60</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="5"/>
+      <c r="E14" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="3">
+      <c r="G14" s="3">
         <v>6</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="3">
+      <c r="I14" s="3">
         <v>0</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="J14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="K14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="L14" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13">
       <c r="A15" s="5" t="s">
         <v>49</v>
       </c>
@@ -2044,34 +2114,37 @@
         <v>65</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F15" s="3">
+      <c r="G15" s="3">
         <v>17</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="3">
+      <c r="I15" s="3">
         <v>47</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="J15" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="K15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="L15" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="A16" s="5" t="s">
         <v>53</v>
       </c>
@@ -2079,34 +2152,37 @@
         <v>79</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H16" s="3">
+      <c r="I16" s="3">
         <v>45</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="K16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="L16" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:12">
       <c r="A17" s="5" t="s">
         <v>55</v>
       </c>
@@ -2114,217 +2190,231 @@
         <v>86</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F17" s="3">
+      <c r="G17" s="3">
         <v>5</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H17" s="3">
+      <c r="I17" s="3">
         <v>1</v>
       </c>
-      <c r="I17" s="4">
+      <c r="J17" s="4">
         <v>45182</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="K17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="L17" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:12">
       <c r="A18" s="6" t="s">
         <v>106</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F18" s="3">
+      <c r="G18" s="3">
         <v>3</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H18" s="3">
+      <c r="I18" s="3">
         <v>20</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="J18" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="K18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="L18" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:12">
       <c r="A19" s="6" t="s">
         <v>114</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="E19" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F19" s="3">
+      <c r="G19" s="3">
         <v>3</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H19" s="3">
+      <c r="I19" s="3">
         <v>20</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="J19" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="K19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="L19" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:12">
       <c r="A20" s="6" t="s">
         <v>116</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F20" s="3">
+      <c r="G20" s="3">
         <v>3</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H20" s="3">
+      <c r="I20" s="3">
         <v>20</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="J20" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="K20" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="L20" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:12">
       <c r="A21" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F21" s="3">
+      <c r="G21" s="3">
         <v>33</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="H21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="3">
+      <c r="I21" s="3">
         <v>13</v>
       </c>
-      <c r="I21" s="4">
+      <c r="J21" s="4">
         <v>45117</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="K21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="L21" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:12">
       <c r="A22" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="5"/>
+      <c r="D22" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F22" s="3">
+      <c r="G22" s="3">
         <v>42</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="3">
+      <c r="I22" s="3">
         <v>14</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="J22" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="K22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="L22" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="C25" s="5"/>
+    <row r="24" spans="1:12">
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="D25" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="A2:K25">
-    <sortCondition ref="G1:G25"/>
+  <sortState ref="A2:L25">
+    <sortCondition ref="H1:H25"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" display="https://app.gorilla.sc/admin/experiment/142252" xr:uid="{D33890EC-403A-764C-8E6B-C725D9BE6A07}"/>
@@ -2361,12 +2451,12 @@
     <hyperlink ref="B7" r:id="rId32" display="https://app.gorilla.sc/admin/experiment/143025" xr:uid="{9DF6AA2C-DBFD-2B4F-B303-3E7989AEDAEC}"/>
     <hyperlink ref="A15" r:id="rId33" xr:uid="{FBAEFCCD-AFE0-E544-9D5B-021BC224BDBA}"/>
     <hyperlink ref="A22" r:id="rId34" xr:uid="{120B1E88-1C4D-6A41-9FDE-B62B36B05308}"/>
-    <hyperlink ref="D18" r:id="rId35" xr:uid="{46FD669D-3543-5347-9B69-6A8A7C2542D8}"/>
+    <hyperlink ref="E18" r:id="rId35" xr:uid="{46FD669D-3543-5347-9B69-6A8A7C2542D8}"/>
     <hyperlink ref="A18" r:id="rId36" xr:uid="{C3B7567D-90E0-D447-ABA3-86042F18C72E}"/>
     <hyperlink ref="B18" r:id="rId37" xr:uid="{F7876E38-8B28-E64C-BD43-8BA1D23A4B96}"/>
     <hyperlink ref="B17" r:id="rId38" display="https://app.gorilla.sc/admin/experiment/143018" xr:uid="{9F128445-1BDD-814A-9B65-8F18DAF8B76D}"/>
     <hyperlink ref="A17" r:id="rId39" display="https://app.gorilla.sc/admin/project/105102" xr:uid="{B75F35D7-3BCC-0547-BB45-DEB230D5F30A}"/>
-    <hyperlink ref="D20" r:id="rId40" xr:uid="{EB94B830-4844-BD4A-B600-44C398D69267}"/>
+    <hyperlink ref="E20" r:id="rId40" xr:uid="{EB94B830-4844-BD4A-B600-44C398D69267}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2376,8 +2466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEF90CF-4CB5-8A43-AC17-CCF9610BD222}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3538,7 +3628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0EBF7F-DB98-AC42-941C-7C09939411EE}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -3730,10 +3820,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C34846-31F7-6D4F-84C1-025AA01B057C}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3850,6 +3940,23 @@
       </c>
       <c r="P2" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>343</v>
+      </c>
+      <c r="B3" t="s">
+        <v>343</v>
+      </c>
+      <c r="C3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E3" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -4124,16 +4231,16 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7586151B-4E7D-4418-B659-2C4EEEFAD5DD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="47378dc1-fef5-4e17-a461-02e6a7c158f1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="e5a9619a-7000-4aea-a2bb-374d291ba315"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>